<commit_message>
IPC  Dist for Mobilzation cost
IPC  Dist for Mobilzation cost
</commit_message>
<xml_diff>
--- a/Civilworks cost/RADP Preparations/Projecttion_output.xlsx
+++ b/Civilworks cost/RADP Preparations/Projecttion_output.xlsx
@@ -22,12 +22,12 @@
     <sheet name="Package_wise_str_value" sheetId="8" r:id="rId8"/>
     <sheet name="Package_wise_str_df" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3082" uniqueCount="468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3091" uniqueCount="468">
   <si>
     <t>Items</t>
   </si>
@@ -1506,13 +1506,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1820,9 +1826,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15:C16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="20.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
@@ -29052,6 +29063,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="12.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
@@ -31830,91 +31844,76 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R47"/>
+  <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="O37" sqref="O37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.44140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" customWidth="1"/>
+    <col min="8" max="8" width="10" customWidth="1"/>
+    <col min="9" max="9" width="8.6640625" customWidth="1"/>
+    <col min="10" max="10" width="10.109375" customWidth="1"/>
+    <col min="11" max="11" width="14.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:11" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>460</v>
       </c>
-      <c r="B1" s="1">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1">
-        <v>14</v>
-      </c>
-      <c r="P1" s="1">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="1">
-        <v>16</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>384</v>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
+      <c r="B2" s="2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2">
         <v>9.0200000000000002E-2</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
         <v>0</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>0.90980000000000005</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -31923,51 +31922,30 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <v>0.90980000000000005</v>
+        <v>0</v>
       </c>
       <c r="J2">
         <v>0</v>
       </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="R2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="K2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
+      <c r="B3" s="2">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2">
         <v>0.35920000000000002</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>0.60660000000000003</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -31976,50 +31954,29 @@
         <v>0</v>
       </c>
       <c r="H3">
-        <v>0.60660000000000003</v>
+        <v>0</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>3.4200000000000001E-2</v>
       </c>
       <c r="J3">
         <v>0</v>
       </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>3.4200000000000001E-2</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
-      <c r="P3">
-        <v>0</v>
-      </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-      <c r="R3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="K3" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
+      <c r="B4" s="2">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2">
         <v>0.22559999999999999</v>
       </c>
       <c r="E4">
@@ -32035,47 +31992,26 @@
         <v>0</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>0.77439999999999998</v>
       </c>
       <c r="J4">
         <v>0</v>
       </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>0.77439999999999998</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
-      <c r="R4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="K4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
+      <c r="B5" s="2">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2">
         <v>0.63849999999999996</v>
       </c>
       <c r="E5">
@@ -32091,47 +32027,26 @@
         <v>0</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>0.36149999999999999</v>
       </c>
       <c r="J5">
         <v>0</v>
       </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>0.36149999999999999</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
-      <c r="O5">
-        <v>0</v>
-      </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
-      <c r="Q5">
-        <v>0</v>
-      </c>
-      <c r="R5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="K5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>388</v>
       </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
+      <c r="B6" s="2">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2">
         <v>0.24779999999999999</v>
       </c>
       <c r="E6">
@@ -32147,51 +32062,30 @@
         <v>0</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <v>0.75219999999999998</v>
       </c>
       <c r="J6">
         <v>0</v>
       </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>0.75219999999999998</v>
-      </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
-      <c r="O6">
-        <v>0</v>
-      </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
-      <c r="Q6">
-        <v>0</v>
-      </c>
-      <c r="R6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="K6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
+      <c r="B7" s="2">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2">
         <v>0.29420000000000002</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>0.70579999999999998</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -32200,7 +32094,7 @@
         <v>0</v>
       </c>
       <c r="H7">
-        <v>0.70579999999999998</v>
+        <v>0</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -32208,46 +32102,25 @@
       <c r="J7">
         <v>0</v>
       </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
-      <c r="M7">
-        <v>0</v>
-      </c>
-      <c r="N7">
-        <v>0</v>
-      </c>
-      <c r="O7">
-        <v>0</v>
-      </c>
-      <c r="P7">
-        <v>0</v>
-      </c>
-      <c r="Q7">
-        <v>0</v>
-      </c>
-      <c r="R7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="K7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>390</v>
       </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
+      <c r="B8" s="2">
+        <v>0</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2">
         <v>0</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>0.91379999999999995</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -32256,57 +32129,36 @@
         <v>0</v>
       </c>
       <c r="H8">
-        <v>0.91379999999999995</v>
+        <v>0</v>
       </c>
       <c r="I8">
-        <v>0</v>
+        <v>8.6199999999999999E-2</v>
       </c>
       <c r="J8">
         <v>0</v>
       </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <v>8.6199999999999999E-2</v>
-      </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-      <c r="N8">
-        <v>0</v>
-      </c>
-      <c r="O8">
-        <v>0</v>
-      </c>
-      <c r="P8">
-        <v>0</v>
-      </c>
-      <c r="Q8">
-        <v>0</v>
-      </c>
-      <c r="R8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="K8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>0.55549999999999999</v>
+      <c r="B9" s="2">
+        <v>0</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
       <c r="F9">
-        <v>0.44450000000000001</v>
+        <v>0</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -32320,42 +32172,21 @@
       <c r="J9">
         <v>0</v>
       </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9">
-        <v>0</v>
-      </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
-      <c r="N9">
-        <v>0</v>
-      </c>
-      <c r="O9">
-        <v>0</v>
-      </c>
-      <c r="P9">
-        <v>0</v>
-      </c>
-      <c r="Q9">
-        <v>0</v>
-      </c>
-      <c r="R9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="K9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
+      <c r="B10" s="2">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2">
         <v>0.3009</v>
       </c>
       <c r="E10">
@@ -32371,47 +32202,26 @@
         <v>0</v>
       </c>
       <c r="I10">
-        <v>0</v>
+        <v>0.69910000000000005</v>
       </c>
       <c r="J10">
         <v>0</v>
       </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10">
-        <v>0.69910000000000005</v>
-      </c>
-      <c r="M10">
-        <v>0</v>
-      </c>
-      <c r="N10">
-        <v>0</v>
-      </c>
-      <c r="O10">
-        <v>0</v>
-      </c>
-      <c r="P10">
-        <v>0</v>
-      </c>
-      <c r="Q10">
-        <v>0</v>
-      </c>
-      <c r="R10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="K10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>393</v>
       </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
+      <c r="B11" s="2">
+        <v>0</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2">
         <v>0.32990000000000003</v>
       </c>
       <c r="E11">
@@ -32427,51 +32237,30 @@
         <v>0</v>
       </c>
       <c r="I11">
-        <v>0</v>
+        <v>0.67010000000000003</v>
       </c>
       <c r="J11">
         <v>0</v>
       </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11">
-        <v>0.67010000000000003</v>
-      </c>
-      <c r="M11">
-        <v>0</v>
-      </c>
-      <c r="N11">
-        <v>0</v>
-      </c>
-      <c r="O11">
-        <v>0</v>
-      </c>
-      <c r="P11">
-        <v>0</v>
-      </c>
-      <c r="Q11">
-        <v>0</v>
-      </c>
-      <c r="R11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="K11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>394</v>
       </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
+      <c r="B12" s="2">
+        <v>0</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0</v>
+      </c>
+      <c r="D12" s="2">
         <v>0.56989999999999996</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>0.43009999999999998</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -32480,7 +32269,7 @@
         <v>0</v>
       </c>
       <c r="H12">
-        <v>0.43009999999999998</v>
+        <v>0</v>
       </c>
       <c r="I12">
         <v>0</v>
@@ -32488,42 +32277,21 @@
       <c r="J12">
         <v>0</v>
       </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-      <c r="L12">
-        <v>0</v>
-      </c>
-      <c r="M12">
-        <v>0</v>
-      </c>
-      <c r="N12">
-        <v>0</v>
-      </c>
-      <c r="O12">
-        <v>0</v>
-      </c>
-      <c r="P12">
-        <v>0</v>
-      </c>
-      <c r="Q12">
-        <v>0</v>
-      </c>
-      <c r="R12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="K12" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>395</v>
       </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
+      <c r="B13" s="2">
+        <v>0</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2">
         <v>0.42480000000000001</v>
       </c>
       <c r="E13">
@@ -32539,47 +32307,26 @@
         <v>0</v>
       </c>
       <c r="I13">
-        <v>0</v>
+        <v>0.57520000000000004</v>
       </c>
       <c r="J13">
         <v>0</v>
       </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-      <c r="L13">
-        <v>0.57520000000000004</v>
-      </c>
-      <c r="M13">
-        <v>0</v>
-      </c>
-      <c r="N13">
-        <v>0</v>
-      </c>
-      <c r="O13">
-        <v>0</v>
-      </c>
-      <c r="P13">
-        <v>0</v>
-      </c>
-      <c r="Q13">
-        <v>0</v>
-      </c>
-      <c r="R13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="K13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>396</v>
       </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
+      <c r="B14" s="2">
+        <v>0</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2">
         <v>0.20599999999999999</v>
       </c>
       <c r="E14">
@@ -32595,47 +32342,26 @@
         <v>0</v>
       </c>
       <c r="I14">
-        <v>0</v>
+        <v>0.79400000000000004</v>
       </c>
       <c r="J14">
         <v>0</v>
       </c>
-      <c r="K14">
-        <v>0</v>
-      </c>
-      <c r="L14">
-        <v>0.79400000000000004</v>
-      </c>
-      <c r="M14">
-        <v>0</v>
-      </c>
-      <c r="N14">
-        <v>0</v>
-      </c>
-      <c r="O14">
-        <v>0</v>
-      </c>
-      <c r="P14">
-        <v>0</v>
-      </c>
-      <c r="Q14">
-        <v>0</v>
-      </c>
-      <c r="R14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="K14" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
+      <c r="B15" s="2">
+        <v>0</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0</v>
+      </c>
+      <c r="D15" s="2">
         <v>0.21290000000000001</v>
       </c>
       <c r="E15">
@@ -32651,47 +32377,26 @@
         <v>0</v>
       </c>
       <c r="I15">
-        <v>0</v>
+        <v>0.78710000000000002</v>
       </c>
       <c r="J15">
         <v>0</v>
       </c>
-      <c r="K15">
-        <v>0</v>
-      </c>
-      <c r="L15">
-        <v>0.78710000000000002</v>
-      </c>
-      <c r="M15">
-        <v>0</v>
-      </c>
-      <c r="N15">
-        <v>0</v>
-      </c>
-      <c r="O15">
-        <v>0</v>
-      </c>
-      <c r="P15">
-        <v>0</v>
-      </c>
-      <c r="Q15">
-        <v>0</v>
-      </c>
-      <c r="R15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="K15" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>398</v>
       </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-      <c r="D16">
+      <c r="B16" s="2">
+        <v>0</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0</v>
+      </c>
+      <c r="D16" s="2">
         <v>0.34379999999999999</v>
       </c>
       <c r="E16">
@@ -32707,51 +32412,30 @@
         <v>0</v>
       </c>
       <c r="I16">
-        <v>0</v>
+        <v>0.65620000000000001</v>
       </c>
       <c r="J16">
         <v>0</v>
       </c>
-      <c r="K16">
-        <v>0</v>
-      </c>
-      <c r="L16">
-        <v>0.65620000000000001</v>
-      </c>
-      <c r="M16">
-        <v>0</v>
-      </c>
-      <c r="N16">
-        <v>0</v>
-      </c>
-      <c r="O16">
-        <v>0</v>
-      </c>
-      <c r="P16">
-        <v>0</v>
-      </c>
-      <c r="Q16">
-        <v>0</v>
-      </c>
-      <c r="R16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="K16" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>399</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="2">
         <v>0.17499999999999999</v>
       </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17">
-        <v>0.36109999999999998</v>
+      <c r="C17" s="2">
+        <v>0</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0.47429999999999994</v>
       </c>
       <c r="E17">
-        <v>0.1132</v>
+        <v>0</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -32763,60 +32447,39 @@
         <v>0</v>
       </c>
       <c r="I17">
-        <v>0</v>
+        <v>0.3508</v>
       </c>
       <c r="J17">
         <v>0</v>
       </c>
-      <c r="K17">
-        <v>0</v>
-      </c>
-      <c r="L17">
-        <v>0.3508</v>
-      </c>
-      <c r="M17">
-        <v>0</v>
-      </c>
-      <c r="N17">
-        <v>0</v>
-      </c>
-      <c r="O17">
-        <v>0</v>
-      </c>
-      <c r="P17">
-        <v>0</v>
-      </c>
-      <c r="Q17">
-        <v>0</v>
-      </c>
-      <c r="R17">
-        <v>1.0001</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="K17" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="B18">
-        <v>0</v>
-      </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
+      <c r="B18" s="2">
+        <v>0</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.58799999999999997</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>0.41199999999999998</v>
       </c>
       <c r="F18">
-        <v>0.58799999999999997</v>
+        <v>0</v>
       </c>
       <c r="G18">
         <v>0</v>
       </c>
       <c r="H18">
-        <v>0.41199999999999998</v>
+        <v>0</v>
       </c>
       <c r="I18">
         <v>0</v>
@@ -32824,46 +32487,25 @@
       <c r="J18">
         <v>0</v>
       </c>
-      <c r="K18">
-        <v>0</v>
-      </c>
-      <c r="L18">
-        <v>0</v>
-      </c>
-      <c r="M18">
-        <v>0</v>
-      </c>
-      <c r="N18">
-        <v>0</v>
-      </c>
-      <c r="O18">
-        <v>0</v>
-      </c>
-      <c r="P18">
-        <v>0</v>
-      </c>
-      <c r="Q18">
-        <v>0</v>
-      </c>
-      <c r="R18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="K18" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>401</v>
       </c>
-      <c r="B19">
-        <v>0</v>
-      </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-      <c r="D19">
+      <c r="B19" s="2">
+        <v>0</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0</v>
+      </c>
+      <c r="D19" s="2">
         <v>0</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19">
         <v>0</v>
@@ -32872,7 +32514,7 @@
         <v>0</v>
       </c>
       <c r="H19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I19">
         <v>0</v>
@@ -32880,49 +32522,28 @@
       <c r="J19">
         <v>0</v>
       </c>
-      <c r="K19">
-        <v>0</v>
-      </c>
-      <c r="L19">
-        <v>0</v>
-      </c>
-      <c r="M19">
-        <v>0</v>
-      </c>
-      <c r="N19">
-        <v>0</v>
-      </c>
-      <c r="O19">
-        <v>0</v>
-      </c>
-      <c r="P19">
-        <v>0</v>
-      </c>
-      <c r="Q19">
-        <v>0</v>
-      </c>
-      <c r="R19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="K19" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>402</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="2">
         <v>0.28970000000000001</v>
       </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="D20">
-        <v>0.1454</v>
+      <c r="C20" s="2">
+        <v>0</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0.71029999999999993</v>
       </c>
       <c r="E20">
         <v>0</v>
       </c>
       <c r="F20">
-        <v>0.56489999999999996</v>
+        <v>0</v>
       </c>
       <c r="G20">
         <v>0</v>
@@ -32936,42 +32557,21 @@
       <c r="J20">
         <v>0</v>
       </c>
-      <c r="K20">
-        <v>0</v>
-      </c>
-      <c r="L20">
-        <v>0</v>
-      </c>
-      <c r="M20">
-        <v>0</v>
-      </c>
-      <c r="N20">
-        <v>0</v>
-      </c>
-      <c r="O20">
-        <v>0</v>
-      </c>
-      <c r="P20">
-        <v>0</v>
-      </c>
-      <c r="Q20">
-        <v>0</v>
-      </c>
-      <c r="R20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="K20" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>403</v>
       </c>
-      <c r="B21">
-        <v>0</v>
-      </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-      <c r="D21">
+      <c r="B21" s="2">
+        <v>0</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0</v>
+      </c>
+      <c r="D21" s="2">
         <v>0.51529999999999998</v>
       </c>
       <c r="E21">
@@ -32987,107 +32587,65 @@
         <v>0</v>
       </c>
       <c r="I21">
-        <v>0</v>
+        <v>0.35470000000000002</v>
       </c>
       <c r="J21">
-        <v>0</v>
-      </c>
-      <c r="K21">
-        <v>0</v>
-      </c>
-      <c r="L21">
-        <v>0.35470000000000002</v>
-      </c>
-      <c r="M21">
         <v>0.12989999999999999</v>
       </c>
-      <c r="N21">
-        <v>0</v>
-      </c>
-      <c r="O21">
-        <v>0</v>
-      </c>
-      <c r="P21">
-        <v>0</v>
-      </c>
-      <c r="Q21">
-        <v>0</v>
-      </c>
-      <c r="R21">
-        <v>0.99990000000000001</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="K21" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="B22">
-        <v>0</v>
-      </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
+      <c r="B22" s="2">
+        <v>0</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0.42399999999999999</v>
       </c>
       <c r="E22">
-        <v>0.15279999999999999</v>
+        <v>0.24809999999999999</v>
       </c>
       <c r="F22">
-        <v>0.2712</v>
+        <v>0</v>
       </c>
       <c r="G22">
         <v>0</v>
       </c>
       <c r="H22">
-        <v>0.24809999999999999</v>
+        <v>0</v>
       </c>
       <c r="I22">
-        <v>0</v>
+        <v>0.32790000000000002</v>
       </c>
       <c r="J22">
         <v>0</v>
       </c>
-      <c r="K22">
-        <v>0</v>
-      </c>
-      <c r="L22">
-        <v>0.32790000000000002</v>
-      </c>
-      <c r="M22">
-        <v>0</v>
-      </c>
-      <c r="N22">
-        <v>0</v>
-      </c>
-      <c r="O22">
-        <v>0</v>
-      </c>
-      <c r="P22">
-        <v>0</v>
-      </c>
-      <c r="Q22">
-        <v>0</v>
-      </c>
-      <c r="R22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="K22" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>405</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="2">
         <v>8.2299999999999998E-2</v>
       </c>
-      <c r="C23">
-        <v>0</v>
-      </c>
-      <c r="D23">
-        <v>0.68379999999999996</v>
+      <c r="C23" s="2">
+        <v>0</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0.73469999999999991</v>
       </c>
       <c r="E23">
-        <v>5.0900000000000001E-2</v>
+        <v>4.24E-2</v>
       </c>
       <c r="F23">
         <v>0</v>
@@ -33096,50 +32654,29 @@
         <v>0</v>
       </c>
       <c r="H23">
-        <v>4.24E-2</v>
+        <v>0</v>
       </c>
       <c r="I23">
-        <v>0</v>
+        <v>0.1406</v>
       </c>
       <c r="J23">
         <v>0</v>
       </c>
-      <c r="K23">
-        <v>0</v>
-      </c>
-      <c r="L23">
-        <v>0.1406</v>
-      </c>
-      <c r="M23">
-        <v>0</v>
-      </c>
-      <c r="N23">
-        <v>0</v>
-      </c>
-      <c r="O23">
-        <v>0</v>
-      </c>
-      <c r="P23">
-        <v>0</v>
-      </c>
-      <c r="Q23">
-        <v>0</v>
-      </c>
-      <c r="R23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="K23" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="B24">
-        <v>0</v>
-      </c>
-      <c r="C24">
-        <v>0</v>
-      </c>
-      <c r="D24">
+      <c r="B24" s="2">
+        <v>0</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0</v>
+      </c>
+      <c r="D24" s="2">
         <v>0</v>
       </c>
       <c r="E24">
@@ -33155,60 +32692,39 @@
         <v>0</v>
       </c>
       <c r="I24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J24">
         <v>0</v>
       </c>
-      <c r="K24">
-        <v>0</v>
-      </c>
-      <c r="L24">
-        <v>1</v>
-      </c>
-      <c r="M24">
-        <v>0</v>
-      </c>
-      <c r="N24">
-        <v>0</v>
-      </c>
-      <c r="O24">
-        <v>0</v>
-      </c>
-      <c r="P24">
-        <v>0</v>
-      </c>
-      <c r="Q24">
-        <v>0</v>
-      </c>
-      <c r="R24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="K24" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="2">
         <v>6.7199999999999996E-2</v>
       </c>
-      <c r="C25">
-        <v>0</v>
-      </c>
-      <c r="D25">
-        <v>0.23</v>
+      <c r="C25" s="2">
+        <v>0</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.72060000000000002</v>
       </c>
       <c r="E25">
-        <v>2.3699999999999999E-2</v>
+        <v>0.2122</v>
       </c>
       <c r="F25">
-        <v>0.46689999999999998</v>
+        <v>0</v>
       </c>
       <c r="G25">
         <v>0</v>
       </c>
       <c r="H25">
-        <v>0.2122</v>
+        <v>0</v>
       </c>
       <c r="I25">
         <v>0</v>
@@ -33216,46 +32732,25 @@
       <c r="J25">
         <v>0</v>
       </c>
-      <c r="K25">
-        <v>0</v>
-      </c>
-      <c r="L25">
-        <v>0</v>
-      </c>
-      <c r="M25">
-        <v>0</v>
-      </c>
-      <c r="N25">
-        <v>0</v>
-      </c>
-      <c r="O25">
-        <v>0</v>
-      </c>
-      <c r="P25">
-        <v>0</v>
-      </c>
-      <c r="Q25">
-        <v>0</v>
-      </c>
-      <c r="R25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="K25" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="B26">
-        <v>0</v>
-      </c>
-      <c r="C26">
-        <v>0</v>
-      </c>
-      <c r="D26">
+      <c r="B26" s="2">
+        <v>0</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0</v>
+      </c>
+      <c r="D26" s="2">
         <v>0</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>0.95369999999999999</v>
       </c>
       <c r="F26">
         <v>0</v>
@@ -33264,57 +32759,36 @@
         <v>0</v>
       </c>
       <c r="H26">
-        <v>0.95369999999999999</v>
+        <v>0</v>
       </c>
       <c r="I26">
-        <v>0</v>
+        <v>4.6300000000000001E-2</v>
       </c>
       <c r="J26">
         <v>0</v>
       </c>
-      <c r="K26">
-        <v>0</v>
-      </c>
-      <c r="L26">
-        <v>4.6300000000000001E-2</v>
-      </c>
-      <c r="M26">
-        <v>0</v>
-      </c>
-      <c r="N26">
-        <v>0</v>
-      </c>
-      <c r="O26">
-        <v>0</v>
-      </c>
-      <c r="P26">
-        <v>0</v>
-      </c>
-      <c r="Q26">
-        <v>0</v>
-      </c>
-      <c r="R26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="K26" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>409</v>
       </c>
-      <c r="B27">
-        <v>0</v>
-      </c>
-      <c r="C27">
-        <v>0</v>
-      </c>
-      <c r="D27">
-        <v>0.34050000000000002</v>
+      <c r="B27" s="2">
+        <v>0</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0</v>
+      </c>
+      <c r="D27" s="2">
+        <v>1</v>
       </c>
       <c r="E27">
-        <v>4.6800000000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="F27">
-        <v>0.61270000000000002</v>
+        <v>0</v>
       </c>
       <c r="G27">
         <v>0</v>
@@ -33328,42 +32802,21 @@
       <c r="J27">
         <v>0</v>
       </c>
-      <c r="K27">
-        <v>0</v>
-      </c>
-      <c r="L27">
-        <v>0</v>
-      </c>
-      <c r="M27">
-        <v>0</v>
-      </c>
-      <c r="N27">
-        <v>0</v>
-      </c>
-      <c r="O27">
-        <v>0</v>
-      </c>
-      <c r="P27">
-        <v>0</v>
-      </c>
-      <c r="Q27">
-        <v>0</v>
-      </c>
-      <c r="R27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="K27" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>410</v>
       </c>
-      <c r="B28">
-        <v>0</v>
-      </c>
-      <c r="C28">
-        <v>0</v>
-      </c>
-      <c r="D28">
+      <c r="B28" s="2">
+        <v>0</v>
+      </c>
+      <c r="C28" s="2">
+        <v>0</v>
+      </c>
+      <c r="D28" s="2">
         <v>0</v>
       </c>
       <c r="E28">
@@ -33373,7 +32826,7 @@
         <v>0</v>
       </c>
       <c r="G28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H28">
         <v>0</v>
@@ -33382,51 +32835,30 @@
         <v>0</v>
       </c>
       <c r="J28">
-        <v>1</v>
-      </c>
-      <c r="K28">
-        <v>0</v>
-      </c>
-      <c r="L28">
-        <v>0</v>
-      </c>
-      <c r="M28">
-        <v>0</v>
-      </c>
-      <c r="N28">
-        <v>0</v>
-      </c>
-      <c r="O28">
-        <v>0</v>
-      </c>
-      <c r="P28">
-        <v>0</v>
-      </c>
-      <c r="Q28">
-        <v>0</v>
-      </c>
-      <c r="R28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="K28" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>411</v>
       </c>
-      <c r="B29">
-        <v>0</v>
-      </c>
-      <c r="C29">
-        <v>0</v>
-      </c>
-      <c r="D29">
+      <c r="B29" s="2">
+        <v>0</v>
+      </c>
+      <c r="C29" s="2">
+        <v>0</v>
+      </c>
+      <c r="D29" s="2">
         <v>0</v>
       </c>
       <c r="E29">
         <v>0</v>
       </c>
       <c r="F29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G29">
         <v>0</v>
@@ -33435,47 +32867,26 @@
         <v>0</v>
       </c>
       <c r="I29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J29">
         <v>0</v>
       </c>
-      <c r="K29">
-        <v>0</v>
-      </c>
-      <c r="L29">
-        <v>0</v>
-      </c>
-      <c r="M29">
-        <v>0</v>
-      </c>
-      <c r="N29">
-        <v>0</v>
-      </c>
-      <c r="O29">
-        <v>0</v>
-      </c>
-      <c r="P29">
-        <v>0</v>
-      </c>
-      <c r="Q29">
-        <v>0</v>
-      </c>
-      <c r="R29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="K29" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="B30">
-        <v>0</v>
-      </c>
-      <c r="C30">
+      <c r="B30" s="2">
+        <v>0</v>
+      </c>
+      <c r="C30" s="2">
         <v>0.44829999999999998</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="2">
         <v>0</v>
       </c>
       <c r="E30">
@@ -33485,109 +32896,67 @@
         <v>0</v>
       </c>
       <c r="G30">
-        <v>0</v>
+        <v>0.5181</v>
       </c>
       <c r="H30">
-        <v>0</v>
+        <v>3.3599999999999998E-2</v>
       </c>
       <c r="I30">
         <v>0</v>
       </c>
       <c r="J30">
-        <v>0.5181</v>
-      </c>
-      <c r="K30">
-        <v>3.3599999999999998E-2</v>
-      </c>
-      <c r="L30">
-        <v>0</v>
-      </c>
-      <c r="M30">
-        <v>0</v>
-      </c>
-      <c r="N30">
-        <v>0</v>
-      </c>
-      <c r="O30">
-        <v>0</v>
-      </c>
-      <c r="P30">
-        <v>0</v>
-      </c>
-      <c r="Q30">
-        <v>0</v>
-      </c>
-      <c r="R30">
-        <v>0.99999999999999989</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="K30" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>413</v>
       </c>
-      <c r="B31">
-        <v>0</v>
-      </c>
-      <c r="C31">
-        <v>0</v>
-      </c>
-      <c r="D31">
+      <c r="B31" s="2">
+        <v>0</v>
+      </c>
+      <c r="C31" s="2">
+        <v>0</v>
+      </c>
+      <c r="D31" s="2">
         <v>0</v>
       </c>
       <c r="E31">
         <v>0</v>
       </c>
       <c r="F31">
-        <v>0</v>
+        <v>0.73640000000000005</v>
       </c>
       <c r="G31">
         <v>0</v>
       </c>
       <c r="H31">
-        <v>0</v>
+        <v>0.2636</v>
       </c>
       <c r="I31">
-        <v>0.73640000000000005</v>
+        <v>0</v>
       </c>
       <c r="J31">
         <v>0</v>
       </c>
-      <c r="K31">
-        <v>0.2636</v>
-      </c>
-      <c r="L31">
-        <v>0</v>
-      </c>
-      <c r="M31">
-        <v>0</v>
-      </c>
-      <c r="N31">
-        <v>0</v>
-      </c>
-      <c r="O31">
-        <v>0</v>
-      </c>
-      <c r="P31">
-        <v>0</v>
-      </c>
-      <c r="Q31">
-        <v>0</v>
-      </c>
-      <c r="R31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="K31" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="B32">
-        <v>0</v>
-      </c>
-      <c r="C32">
-        <v>0</v>
-      </c>
-      <c r="D32">
+      <c r="B32" s="2">
+        <v>0</v>
+      </c>
+      <c r="C32" s="2">
+        <v>0</v>
+      </c>
+      <c r="D32" s="2">
         <v>0.95189999999999997</v>
       </c>
       <c r="E32">
@@ -33600,7 +32969,7 @@
         <v>0</v>
       </c>
       <c r="H32">
-        <v>0</v>
+        <v>4.8099999999999997E-2</v>
       </c>
       <c r="I32">
         <v>0</v>
@@ -33608,46 +32977,25 @@
       <c r="J32">
         <v>0</v>
       </c>
-      <c r="K32">
-        <v>4.8099999999999997E-2</v>
-      </c>
-      <c r="L32">
-        <v>0</v>
-      </c>
-      <c r="M32">
-        <v>0</v>
-      </c>
-      <c r="N32">
-        <v>0</v>
-      </c>
-      <c r="O32">
-        <v>0</v>
-      </c>
-      <c r="P32">
-        <v>0</v>
-      </c>
-      <c r="Q32">
-        <v>0</v>
-      </c>
-      <c r="R32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="K32" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="2">
         <v>2.6800000000000001E-2</v>
       </c>
-      <c r="C33">
-        <v>0</v>
-      </c>
-      <c r="D33">
-        <v>0</v>
+      <c r="C33" s="2">
+        <v>0</v>
+      </c>
+      <c r="D33" s="2">
+        <v>0.1338</v>
       </c>
       <c r="E33">
-        <v>0.1338</v>
+        <v>0.80859999999999999</v>
       </c>
       <c r="F33">
         <v>0</v>
@@ -33656,54 +33004,33 @@
         <v>0</v>
       </c>
       <c r="H33">
-        <v>0.80859999999999999</v>
+        <v>0</v>
       </c>
       <c r="I33">
         <v>0</v>
       </c>
       <c r="J33">
-        <v>0</v>
-      </c>
-      <c r="K33">
-        <v>0</v>
-      </c>
-      <c r="L33">
-        <v>0</v>
-      </c>
-      <c r="M33">
         <v>3.0800000000000001E-2</v>
       </c>
-      <c r="N33">
-        <v>0</v>
-      </c>
-      <c r="O33">
-        <v>0</v>
-      </c>
-      <c r="P33">
-        <v>0</v>
-      </c>
-      <c r="Q33">
-        <v>0</v>
-      </c>
-      <c r="R33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="K33" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>416</v>
       </c>
-      <c r="B34">
-        <v>0</v>
-      </c>
-      <c r="C34">
-        <v>0</v>
-      </c>
-      <c r="D34">
+      <c r="B34" s="2">
+        <v>0</v>
+      </c>
+      <c r="C34" s="2">
+        <v>0</v>
+      </c>
+      <c r="D34" s="2">
         <v>0</v>
       </c>
       <c r="E34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F34">
         <v>0</v>
@@ -33712,7 +33039,7 @@
         <v>0</v>
       </c>
       <c r="H34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I34">
         <v>0</v>
@@ -33720,46 +33047,25 @@
       <c r="J34">
         <v>0</v>
       </c>
-      <c r="K34">
-        <v>0</v>
-      </c>
-      <c r="L34">
-        <v>0</v>
-      </c>
-      <c r="M34">
-        <v>0</v>
-      </c>
-      <c r="N34">
-        <v>0</v>
-      </c>
-      <c r="O34">
-        <v>0</v>
-      </c>
-      <c r="P34">
-        <v>0</v>
-      </c>
-      <c r="Q34">
-        <v>0</v>
-      </c>
-      <c r="R34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="K34" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="2">
         <v>4.1700000000000001E-2</v>
       </c>
-      <c r="C35">
-        <v>0</v>
-      </c>
-      <c r="D35">
-        <v>0.60370000000000001</v>
+      <c r="C35" s="2">
+        <v>0</v>
+      </c>
+      <c r="D35" s="2">
+        <v>0.95830000000000004</v>
       </c>
       <c r="E35">
-        <v>0.35460000000000003</v>
+        <v>0</v>
       </c>
       <c r="F35">
         <v>0</v>
@@ -33776,46 +33082,25 @@
       <c r="J35">
         <v>0</v>
       </c>
-      <c r="K35">
-        <v>0</v>
-      </c>
-      <c r="L35">
-        <v>0</v>
-      </c>
-      <c r="M35">
-        <v>0</v>
-      </c>
-      <c r="N35">
-        <v>0</v>
-      </c>
-      <c r="O35">
-        <v>0</v>
-      </c>
-      <c r="P35">
-        <v>0</v>
-      </c>
-      <c r="Q35">
-        <v>0</v>
-      </c>
-      <c r="R35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="K35" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>424</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="2">
         <v>7.3000000000000001E-3</v>
       </c>
-      <c r="C36">
-        <v>0</v>
-      </c>
-      <c r="D36">
-        <v>0</v>
+      <c r="C36" s="2">
+        <v>0</v>
+      </c>
+      <c r="D36" s="2">
+        <v>0.21590000000000001</v>
       </c>
       <c r="E36">
-        <v>0.21590000000000001</v>
+        <v>0.18360000000000001</v>
       </c>
       <c r="F36">
         <v>0</v>
@@ -33824,54 +33109,33 @@
         <v>0</v>
       </c>
       <c r="H36">
-        <v>0.18360000000000001</v>
+        <v>0</v>
       </c>
       <c r="I36">
-        <v>0</v>
+        <v>0.59319999999999995</v>
       </c>
       <c r="J36">
         <v>0</v>
       </c>
-      <c r="K36">
-        <v>0</v>
-      </c>
-      <c r="L36">
-        <v>0.59319999999999995</v>
-      </c>
-      <c r="M36">
-        <v>0</v>
-      </c>
-      <c r="N36">
-        <v>0</v>
-      </c>
-      <c r="O36">
-        <v>0</v>
-      </c>
-      <c r="P36">
-        <v>0</v>
-      </c>
-      <c r="Q36">
-        <v>0</v>
-      </c>
-      <c r="R36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="K36" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>425</v>
       </c>
-      <c r="B37">
-        <v>0</v>
-      </c>
-      <c r="C37">
-        <v>0</v>
-      </c>
-      <c r="D37">
+      <c r="B37" s="2">
+        <v>0</v>
+      </c>
+      <c r="C37" s="2">
+        <v>0</v>
+      </c>
+      <c r="D37" s="2">
         <v>0</v>
       </c>
       <c r="E37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F37">
         <v>0</v>
@@ -33880,7 +33144,7 @@
         <v>0</v>
       </c>
       <c r="H37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I37">
         <v>0</v>
@@ -33888,49 +33152,28 @@
       <c r="J37">
         <v>0</v>
       </c>
-      <c r="K37">
-        <v>0</v>
-      </c>
-      <c r="L37">
-        <v>0</v>
-      </c>
-      <c r="M37">
-        <v>0</v>
-      </c>
-      <c r="N37">
-        <v>0</v>
-      </c>
-      <c r="O37">
-        <v>0</v>
-      </c>
-      <c r="P37">
-        <v>0</v>
-      </c>
-      <c r="Q37">
-        <v>0</v>
-      </c>
-      <c r="R37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="K37" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>426</v>
       </c>
-      <c r="B38">
-        <v>0</v>
-      </c>
-      <c r="C38">
-        <v>0</v>
-      </c>
-      <c r="D38">
-        <v>0.29210000000000003</v>
+      <c r="B38" s="2">
+        <v>0</v>
+      </c>
+      <c r="C38" s="2">
+        <v>0</v>
+      </c>
+      <c r="D38" s="2">
+        <v>1</v>
       </c>
       <c r="E38">
         <v>0</v>
       </c>
       <c r="F38">
-        <v>0.70789999999999997</v>
+        <v>0</v>
       </c>
       <c r="G38">
         <v>0</v>
@@ -33944,42 +33187,21 @@
       <c r="J38">
         <v>0</v>
       </c>
-      <c r="K38">
-        <v>0</v>
-      </c>
-      <c r="L38">
-        <v>0</v>
-      </c>
-      <c r="M38">
-        <v>0</v>
-      </c>
-      <c r="N38">
-        <v>0</v>
-      </c>
-      <c r="O38">
-        <v>0</v>
-      </c>
-      <c r="P38">
-        <v>0</v>
-      </c>
-      <c r="Q38">
-        <v>0</v>
-      </c>
-      <c r="R38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="K38" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>427</v>
       </c>
-      <c r="B39">
-        <v>0</v>
-      </c>
-      <c r="C39">
-        <v>0</v>
-      </c>
-      <c r="D39">
+      <c r="B39" s="2">
+        <v>0</v>
+      </c>
+      <c r="C39" s="2">
+        <v>0</v>
+      </c>
+      <c r="D39" s="2">
         <v>0</v>
       </c>
       <c r="E39">
@@ -33995,54 +33217,33 @@
         <v>0</v>
       </c>
       <c r="I39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J39">
         <v>0</v>
       </c>
-      <c r="K39">
-        <v>0</v>
-      </c>
-      <c r="L39">
-        <v>1</v>
-      </c>
-      <c r="M39">
-        <v>0</v>
-      </c>
-      <c r="N39">
-        <v>0</v>
-      </c>
-      <c r="O39">
-        <v>0</v>
-      </c>
-      <c r="P39">
-        <v>0</v>
-      </c>
-      <c r="Q39">
-        <v>0</v>
-      </c>
-      <c r="R39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="K39" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="B40">
-        <v>0</v>
-      </c>
-      <c r="C40">
-        <v>0</v>
-      </c>
-      <c r="D40">
-        <v>0.37809999999999999</v>
+      <c r="B40" s="2">
+        <v>0</v>
+      </c>
+      <c r="C40" s="2">
+        <v>0</v>
+      </c>
+      <c r="D40" s="2">
+        <v>1</v>
       </c>
       <c r="E40">
         <v>0</v>
       </c>
       <c r="F40">
-        <v>0.62190000000000001</v>
+        <v>0</v>
       </c>
       <c r="G40">
         <v>0</v>
@@ -34056,46 +33257,25 @@
       <c r="J40">
         <v>0</v>
       </c>
-      <c r="K40">
-        <v>0</v>
-      </c>
-      <c r="L40">
-        <v>0</v>
-      </c>
-      <c r="M40">
-        <v>0</v>
-      </c>
-      <c r="N40">
-        <v>0</v>
-      </c>
-      <c r="O40">
-        <v>0</v>
-      </c>
-      <c r="P40">
-        <v>0</v>
-      </c>
-      <c r="Q40">
-        <v>0</v>
-      </c>
-      <c r="R40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="K40" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>429</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="2">
         <v>8.3299999999999999E-2</v>
       </c>
-      <c r="C41">
-        <v>0</v>
-      </c>
-      <c r="D41">
-        <v>0</v>
+      <c r="C41" s="2">
+        <v>0</v>
+      </c>
+      <c r="D41" s="2">
+        <v>2.86E-2</v>
       </c>
       <c r="E41">
-        <v>2.86E-2</v>
+        <v>0.88800000000000001</v>
       </c>
       <c r="F41">
         <v>0</v>
@@ -34104,7 +33284,7 @@
         <v>0</v>
       </c>
       <c r="H41">
-        <v>0.88800000000000001</v>
+        <v>0</v>
       </c>
       <c r="I41">
         <v>0</v>
@@ -34112,154 +33292,91 @@
       <c r="J41">
         <v>0</v>
       </c>
-      <c r="K41">
-        <v>0</v>
-      </c>
-      <c r="L41">
-        <v>0</v>
-      </c>
-      <c r="M41">
-        <v>0</v>
-      </c>
-      <c r="N41">
-        <v>0</v>
-      </c>
-      <c r="O41">
-        <v>0</v>
-      </c>
-      <c r="P41">
-        <v>0</v>
-      </c>
-      <c r="Q41">
-        <v>0</v>
-      </c>
-      <c r="R41">
-        <v>0.99990000000000001</v>
-      </c>
-    </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="K41" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="B42">
-        <v>0</v>
-      </c>
-      <c r="C42">
-        <v>0</v>
-      </c>
-      <c r="D42">
-        <v>0.13669999999999999</v>
+      <c r="B42" s="2">
+        <v>0</v>
+      </c>
+      <c r="C42" s="2">
+        <v>0</v>
+      </c>
+      <c r="D42" s="2">
+        <v>0.25379999999999997</v>
       </c>
       <c r="E42">
         <v>0</v>
       </c>
       <c r="F42">
-        <v>0.1171</v>
+        <v>0.54720000000000002</v>
       </c>
       <c r="G42">
         <v>0</v>
       </c>
       <c r="H42">
-        <v>0</v>
+        <v>0.19900000000000001</v>
       </c>
       <c r="I42">
-        <v>0.54720000000000002</v>
+        <v>0</v>
       </c>
       <c r="J42">
         <v>0</v>
       </c>
-      <c r="K42">
-        <v>0.19900000000000001</v>
-      </c>
-      <c r="L42">
-        <v>0</v>
-      </c>
-      <c r="M42">
-        <v>0</v>
-      </c>
-      <c r="N42">
-        <v>0</v>
-      </c>
-      <c r="O42">
-        <v>0</v>
-      </c>
-      <c r="P42">
-        <v>0</v>
-      </c>
-      <c r="Q42">
-        <v>0</v>
-      </c>
-      <c r="R42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="K42" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="B43">
-        <v>0</v>
-      </c>
-      <c r="C43">
-        <v>0</v>
-      </c>
-      <c r="D43">
-        <v>0</v>
+      <c r="B43" s="2">
+        <v>0</v>
+      </c>
+      <c r="C43" s="2">
+        <v>0</v>
+      </c>
+      <c r="D43" s="2">
+        <v>0.2215</v>
       </c>
       <c r="E43">
         <v>0</v>
       </c>
       <c r="F43">
-        <v>0.2215</v>
+        <v>0.14199999999999999</v>
       </c>
       <c r="G43">
         <v>0</v>
       </c>
       <c r="H43">
-        <v>0</v>
+        <v>0.63660000000000005</v>
       </c>
       <c r="I43">
-        <v>0.14199999999999999</v>
+        <v>0</v>
       </c>
       <c r="J43">
         <v>0</v>
       </c>
-      <c r="K43">
-        <v>0.63660000000000005</v>
-      </c>
-      <c r="L43">
-        <v>0</v>
-      </c>
-      <c r="M43">
-        <v>0</v>
-      </c>
-      <c r="N43">
-        <v>0</v>
-      </c>
-      <c r="O43">
-        <v>0</v>
-      </c>
-      <c r="P43">
-        <v>0</v>
-      </c>
-      <c r="Q43">
-        <v>0</v>
-      </c>
-      <c r="R43">
-        <v>1.0001</v>
-      </c>
-    </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="K43" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="B44">
-        <v>0</v>
-      </c>
-      <c r="C44">
-        <v>0</v>
-      </c>
-      <c r="D44">
+      <c r="B44" s="2">
+        <v>0</v>
+      </c>
+      <c r="C44" s="2">
+        <v>0</v>
+      </c>
+      <c r="D44" s="2">
         <v>0</v>
       </c>
       <c r="E44">
@@ -34275,47 +33392,26 @@
         <v>0</v>
       </c>
       <c r="I44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J44">
         <v>0</v>
       </c>
-      <c r="K44">
-        <v>0</v>
-      </c>
-      <c r="L44">
-        <v>1</v>
-      </c>
-      <c r="M44">
-        <v>0</v>
-      </c>
-      <c r="N44">
-        <v>0</v>
-      </c>
-      <c r="O44">
-        <v>0</v>
-      </c>
-      <c r="P44">
-        <v>0</v>
-      </c>
-      <c r="Q44">
-        <v>0</v>
-      </c>
-      <c r="R44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="K44" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="B45">
-        <v>0</v>
-      </c>
-      <c r="C45">
-        <v>0</v>
-      </c>
-      <c r="D45">
+      <c r="B45" s="2">
+        <v>0</v>
+      </c>
+      <c r="C45" s="2">
+        <v>0</v>
+      </c>
+      <c r="D45" s="2">
         <v>1</v>
       </c>
       <c r="E45">
@@ -34336,49 +33432,28 @@
       <c r="J45">
         <v>0</v>
       </c>
-      <c r="K45">
-        <v>0</v>
-      </c>
-      <c r="L45">
-        <v>0</v>
-      </c>
-      <c r="M45">
-        <v>0</v>
-      </c>
-      <c r="N45">
-        <v>0</v>
-      </c>
-      <c r="O45">
-        <v>0</v>
-      </c>
-      <c r="P45">
-        <v>0</v>
-      </c>
-      <c r="Q45">
-        <v>0</v>
-      </c>
-      <c r="R45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="K45" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>422</v>
       </c>
-      <c r="B46">
+      <c r="B46" s="2">
         <v>9.5299999999999996E-2</v>
       </c>
-      <c r="C46">
-        <v>0</v>
-      </c>
-      <c r="D46">
-        <v>0</v>
+      <c r="C46" s="2">
+        <v>0</v>
+      </c>
+      <c r="D46" s="2">
+        <v>0.90469999999999995</v>
       </c>
       <c r="E46">
-        <v>0.21099999999999999</v>
+        <v>0</v>
       </c>
       <c r="F46">
-        <v>0.69369999999999998</v>
+        <v>0</v>
       </c>
       <c r="G46">
         <v>0</v>
@@ -34392,46 +33467,25 @@
       <c r="J46">
         <v>0</v>
       </c>
-      <c r="K46">
-        <v>0</v>
-      </c>
-      <c r="L46">
-        <v>0</v>
-      </c>
-      <c r="M46">
-        <v>0</v>
-      </c>
-      <c r="N46">
-        <v>0</v>
-      </c>
-      <c r="O46">
-        <v>0</v>
-      </c>
-      <c r="P46">
-        <v>0</v>
-      </c>
-      <c r="Q46">
-        <v>0</v>
-      </c>
-      <c r="R46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="K46" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="B47">
-        <v>0</v>
-      </c>
-      <c r="C47">
-        <v>0</v>
-      </c>
-      <c r="D47">
+      <c r="B47" s="2">
+        <v>0</v>
+      </c>
+      <c r="C47" s="2">
+        <v>0</v>
+      </c>
+      <c r="D47" s="2">
         <v>0</v>
       </c>
       <c r="E47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F47">
         <v>0</v>
@@ -34440,7 +33494,7 @@
         <v>0</v>
       </c>
       <c r="H47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I47">
         <v>0</v>
@@ -34448,32 +33502,12 @@
       <c r="J47">
         <v>0</v>
       </c>
-      <c r="K47">
-        <v>0</v>
-      </c>
-      <c r="L47">
-        <v>0</v>
-      </c>
-      <c r="M47">
-        <v>0</v>
-      </c>
-      <c r="N47">
-        <v>0</v>
-      </c>
-      <c r="O47">
-        <v>0</v>
-      </c>
-      <c r="P47">
-        <v>0</v>
-      </c>
-      <c r="Q47">
-        <v>0</v>
-      </c>
-      <c r="R47">
-        <v>1</v>
+      <c r="K47" s="2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>